<commit_message>
done with some testcases in luma.com
</commit_message>
<xml_diff>
--- a/com.luma/src/test/resources/test_data.xlsx
+++ b/com.luma/src/test/resources/test_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadou\IdeaProjects\SeleniumBootcamp\com.luma\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\auooz\IdeaProjects\SeleniumBootcamp\com.luma\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B682ED-139F-436E-B51C-72203FBDD0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E64CE1D-4484-4C25-947A-1FB7483BE950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1608" yWindow="1332" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="2" xr2:uid="{63BAD3BA-E091-40CE-9B8C-FA220E697B2E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{63BAD3BA-E091-40CE-9B8C-FA220E697B2E}"/>
   </bookViews>
   <sheets>
     <sheet name="testDoSearch" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>searchterm</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Tees</t>
   </si>
   <si>
-    <t>Bras</t>
-  </si>
-  <si>
     <t>Tanks</t>
   </si>
   <si>
@@ -79,48 +76,12 @@
     <t>password</t>
   </si>
   <si>
-    <t>connie.smith@gmail.com</t>
-  </si>
-  <si>
-    <t>AydenLiam1213</t>
-  </si>
-  <si>
-    <t>connor.smith@gmail.com</t>
-  </si>
-  <si>
-    <t>Ayden1213</t>
-  </si>
-  <si>
     <t>Invalid email address</t>
   </si>
   <si>
     <t>Password</t>
   </si>
   <si>
-    <t>abc1@gmail.com</t>
-  </si>
-  <si>
-    <t>sadouni.dalal@gmail.com</t>
-  </si>
-  <si>
-    <t>roni_cost@example.com</t>
-  </si>
-  <si>
-    <t>roni_cost3@example.com</t>
-  </si>
-  <si>
-    <t>abctestemail2378!!!!@gmail.com</t>
-  </si>
-  <si>
-    <t>QqwertyQ@123!</t>
-  </si>
-  <si>
-    <t>abctestemail2379!!!!@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abctestemail2370!!!!@gmail.com </t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -130,40 +91,64 @@
     <t>Email</t>
   </si>
   <si>
-    <t>abctestemail10@gmail.com</t>
-  </si>
-  <si>
-    <t>abctestemail20@gmail.com</t>
-  </si>
-  <si>
-    <t>abctestemail30@gmail.com</t>
-  </si>
-  <si>
-    <t>Larry</t>
-  </si>
-  <si>
-    <t>Megan</t>
-  </si>
-  <si>
-    <t>Amare</t>
-  </si>
-  <si>
-    <t>Dawson</t>
-  </si>
-  <si>
-    <t>Jones</t>
-  </si>
-  <si>
-    <t>smith</t>
-  </si>
-  <si>
-    <t>abctestemail11@gmail.com</t>
-  </si>
-  <si>
-    <t>abctestemail21@gmail.com</t>
-  </si>
-  <si>
-    <t>abctestemail31@gmail.com</t>
+    <t>goodbook926@gmail.com</t>
+  </si>
+  <si>
+    <t>goodbook936@gmail.com</t>
+  </si>
+  <si>
+    <t>goodbook946@gmail.com</t>
+  </si>
+  <si>
+    <t>GoodBook 1996</t>
+  </si>
+  <si>
+    <t>GoodBook 1997</t>
+  </si>
+  <si>
+    <t>GoodBook1998</t>
+  </si>
+  <si>
+    <t>GoodBook 1998</t>
+  </si>
+  <si>
+    <t>Auooz</t>
+  </si>
+  <si>
+    <t>Ahsan</t>
+  </si>
+  <si>
+    <t>Sadouni</t>
+  </si>
+  <si>
+    <t>Dalal</t>
+  </si>
+  <si>
+    <t>Abdullah</t>
+  </si>
+  <si>
+    <t>Noor</t>
+  </si>
+  <si>
+    <t>nsbchs@kjsbua.jnd</t>
+  </si>
+  <si>
+    <t>amasn@hjg.dmcn</t>
+  </si>
+  <si>
+    <t>njkas2cb@hbcj.sdjkjvn</t>
+  </si>
+  <si>
+    <t>nassjhask897786</t>
+  </si>
+  <si>
+    <t>u86jxkjjbashj</t>
+  </si>
+  <si>
+    <t>kchshds897</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jogger </t>
   </si>
 </sst>
 </file>
@@ -557,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B44960-F352-4FEA-A342-85F04DC89970}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,17 +593,17 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -632,7 +617,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -643,51 +628,43 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -704,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D45730-030E-40CA-907D-93AFB77B716D}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -718,58 +695,58 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -793,42 +770,47 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="2" max="2" width="21.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>15</v>
+      <c r="A2" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>19</v>
+      <c r="A3" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>21</v>
+      <c r="A4" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{FB82CB99-C2A9-431D-916C-2B1617DB257F}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{72C1C930-9A5A-4B3C-BC5C-25CB5857BD5A}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{4CA7D01F-2BC6-4F53-9BEE-A3DD58D5AFDE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -838,7 +820,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -848,22 +830,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>